<commit_message>
2 - mise en place de la base de donnee
</commit_message>
<xml_diff>
--- a/_annexes/Work_Plan_Village_Green_Haja.xlsx
+++ b/_annexes/Work_Plan_Village_Green_Haja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frhaj\Desktop\Village_green_Haja\_annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AE2260-1562-4C3A-B1A0-C018749EBC34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50589E3A-1FC6-494A-A1E5-DC1ADF05BC06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,6 +654,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -671,21 +686,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1043,9 +1043,9 @@
   <dimension ref="A2:AT71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32:B32"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1162,10 +1162,10 @@
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:46" ht="30" customHeight="1">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1300,10 +1300,10 @@
       </c>
     </row>
     <row r="16" spans="1:46" ht="33.75" customHeight="1">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -1350,10 +1350,10 @@
       <c r="AT16" s="15"/>
     </row>
     <row r="17" spans="1:46" ht="32.25" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="20">
         <v>44319</v>
       </c>
@@ -1409,10 +1409,10 @@
       <c r="AT17" s="19"/>
     </row>
     <row r="18" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="44"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="20">
         <v>44319</v>
       </c>
@@ -1468,10 +1468,10 @@
       <c r="AT18" s="19"/>
     </row>
     <row r="19" spans="1:46" ht="36.75" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="20">
         <v>44319</v>
       </c>
@@ -1527,10 +1527,10 @@
       <c r="AT19" s="19"/>
     </row>
     <row r="20" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -1577,10 +1577,10 @@
       <c r="AT20" s="15"/>
     </row>
     <row r="21" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="20">
         <v>44319</v>
       </c>
@@ -1636,10 +1636,10 @@
       <c r="AT21" s="19"/>
     </row>
     <row r="22" spans="1:46" ht="27.75" customHeight="1">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="38"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="20">
         <v>44319</v>
       </c>
@@ -1650,8 +1650,8 @@
         <f>D22-C22</f>
         <v>4</v>
       </c>
-      <c r="F22" s="25" t="s">
-        <v>10</v>
+      <c r="F22" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="34"/>
@@ -1695,10 +1695,10 @@
       <c r="AT22" s="19"/>
     </row>
     <row r="23" spans="1:46" ht="27.75" customHeight="1">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="42"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="20">
         <v>44319</v>
       </c>
@@ -1754,10 +1754,10 @@
       <c r="AT23" s="19"/>
     </row>
     <row r="24" spans="1:46" ht="27.75" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="20">
         <v>44320</v>
       </c>
@@ -1768,8 +1768,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>10</v>
+      <c r="F24" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G24" s="35"/>
       <c r="H24" s="22"/>
@@ -1813,10 +1813,10 @@
       <c r="AT24" s="19"/>
     </row>
     <row r="25" spans="1:46" ht="50.25" customHeight="1">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="42"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="20">
         <v>44320</v>
       </c>
@@ -1827,8 +1827,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="25" t="s">
-        <v>10</v>
+      <c r="F25" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G25" s="35"/>
       <c r="H25" s="22"/>
@@ -1872,10 +1872,10 @@
       <c r="AT25" s="19"/>
     </row>
     <row r="26" spans="1:46" ht="78" customHeight="1">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="42"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="20">
         <v>44321</v>
       </c>
@@ -1886,8 +1886,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="27" t="s">
-        <v>11</v>
+      <c r="F26" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G26" s="35"/>
       <c r="H26" s="34"/>
@@ -1931,10 +1931,10 @@
       <c r="AT26" s="19"/>
     </row>
     <row r="27" spans="1:46" ht="27.75" customHeight="1">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="42"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="20">
         <v>44321</v>
       </c>
@@ -1945,8 +1945,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="27" t="s">
-        <v>11</v>
+      <c r="F27" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G27" s="35"/>
       <c r="H27" s="34"/>
@@ -1990,10 +1990,10 @@
       <c r="AT27" s="19"/>
     </row>
     <row r="28" spans="1:46" ht="31.5" customHeight="1">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="42"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="20">
         <v>44322</v>
       </c>
@@ -2004,8 +2004,8 @@
         <f>D28-C28</f>
         <v>0</v>
       </c>
-      <c r="F28" s="27" t="s">
-        <v>11</v>
+      <c r="F28" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G28" s="35"/>
       <c r="H28" s="34"/>
@@ -2049,10 +2049,10 @@
       <c r="AT28" s="19"/>
     </row>
     <row r="29" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="20">
         <v>44323</v>
       </c>
@@ -2063,8 +2063,8 @@
         <f>D29-C29</f>
         <v>0</v>
       </c>
-      <c r="F29" s="27" t="s">
-        <v>11</v>
+      <c r="F29" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="34"/>
@@ -2108,10 +2108,10 @@
       <c r="AT29" s="19"/>
     </row>
     <row r="30" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -2158,10 +2158,10 @@
       <c r="AT30" s="15"/>
     </row>
     <row r="31" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="20">
         <v>44326</v>
       </c>
@@ -2217,10 +2217,10 @@
       <c r="AT31" s="19"/>
     </row>
     <row r="32" spans="1:46" ht="35.25" customHeight="1">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="20">
         <v>44326</v>
       </c>
@@ -2276,10 +2276,10 @@
       <c r="AT32" s="19"/>
     </row>
     <row r="33" spans="1:46" ht="35.25" customHeight="1">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="42"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="20">
         <v>44326</v>
       </c>
@@ -2335,10 +2335,10 @@
       <c r="AT33" s="19"/>
     </row>
     <row r="34" spans="1:46" ht="39" customHeight="1">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="42"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="20">
         <v>44326</v>
       </c>
@@ -2394,10 +2394,10 @@
       <c r="AT34" s="19"/>
     </row>
     <row r="35" spans="1:46" ht="48" customHeight="1">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="20">
         <v>44327</v>
       </c>
@@ -2453,10 +2453,10 @@
       <c r="AT35" s="19"/>
     </row>
     <row r="36" spans="1:46" ht="32.25" customHeight="1">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="42"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="20">
         <v>44327</v>
       </c>
@@ -2512,10 +2512,10 @@
       <c r="AT36" s="19"/>
     </row>
     <row r="37" spans="1:46" ht="24" customHeight="1">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="42"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="20">
         <v>44327</v>
       </c>
@@ -2571,10 +2571,10 @@
       <c r="AT37" s="19"/>
     </row>
     <row r="38" spans="1:46" ht="24" customHeight="1">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="42"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="20">
         <v>44328</v>
       </c>
@@ -2630,10 +2630,10 @@
       <c r="AT38" s="19"/>
     </row>
     <row r="39" spans="1:46" ht="24" customHeight="1">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="20">
         <v>44328</v>
       </c>
@@ -2644,8 +2644,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F39" s="27" t="s">
-        <v>11</v>
+      <c r="F39" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="G39" s="21"/>
       <c r="H39" s="19"/>
@@ -2689,10 +2689,10 @@
       <c r="AT39" s="19"/>
     </row>
     <row r="40" spans="1:46" ht="34.5" customHeight="1">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="42"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="20">
         <v>44328</v>
       </c>
@@ -2703,8 +2703,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F40" s="27" t="s">
-        <v>11</v>
+      <c r="F40" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="19"/>
@@ -2748,10 +2748,10 @@
       <c r="AT40" s="19"/>
     </row>
     <row r="41" spans="1:46" ht="27" customHeight="1">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="38"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="20">
         <v>44329</v>
       </c>
@@ -2762,8 +2762,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F41" s="27" t="s">
-        <v>11</v>
+      <c r="F41" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="19"/>
@@ -2807,10 +2807,10 @@
       <c r="AT41" s="19"/>
     </row>
     <row r="42" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="42"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="20">
         <v>44329</v>
       </c>
@@ -2821,8 +2821,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F42" s="27" t="s">
-        <v>11</v>
+      <c r="F42" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="G42" s="21"/>
       <c r="H42" s="19"/>
@@ -2866,10 +2866,10 @@
       <c r="AT42" s="19"/>
     </row>
     <row r="43" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="40"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23"/>
       <c r="E43" s="23"/>
@@ -2916,10 +2916,10 @@
       <c r="AT43" s="15"/>
     </row>
     <row r="44" spans="1:46" ht="39" customHeight="1">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="20">
         <v>44333</v>
       </c>
@@ -2975,10 +2975,10 @@
       <c r="AT44" s="19"/>
     </row>
     <row r="45" spans="1:46" ht="38.25" customHeight="1">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="20">
         <v>44334</v>
       </c>
@@ -3034,10 +3034,10 @@
       <c r="AT45" s="19"/>
     </row>
     <row r="46" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="40"/>
+      <c r="B46" s="45"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -3084,10 +3084,10 @@
       <c r="AT46" s="15"/>
     </row>
     <row r="47" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="42"/>
+      <c r="B47" s="47"/>
       <c r="C47" s="20">
         <v>44335</v>
       </c>
@@ -3143,10 +3143,10 @@
       <c r="AT47" s="19"/>
     </row>
     <row r="48" spans="1:46">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="42"/>
+      <c r="B48" s="47"/>
       <c r="C48" s="20">
         <v>44335</v>
       </c>
@@ -3202,10 +3202,10 @@
       <c r="AT48" s="19"/>
     </row>
     <row r="49" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="42"/>
+      <c r="B49" s="47"/>
       <c r="C49" s="20">
         <v>44335</v>
       </c>
@@ -3261,10 +3261,10 @@
       <c r="AT49" s="19"/>
     </row>
     <row r="50" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="20">
         <v>44336</v>
       </c>
@@ -3320,10 +3320,10 @@
       <c r="AT50" s="19"/>
     </row>
     <row r="51" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="42"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="20">
         <v>44336</v>
       </c>
@@ -3379,10 +3379,10 @@
       <c r="AT51" s="19"/>
     </row>
     <row r="52" spans="1:46" ht="33.75" customHeight="1">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="42"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="20">
         <v>44336</v>
       </c>
@@ -3438,10 +3438,10 @@
       <c r="AT52" s="19"/>
     </row>
     <row r="53" spans="1:46" ht="39.75" customHeight="1">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="42"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="20">
         <v>44340</v>
       </c>
@@ -3497,10 +3497,10 @@
       <c r="AT53" s="19"/>
     </row>
     <row r="54" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="38"/>
+      <c r="B54" s="43"/>
       <c r="C54" s="20">
         <v>44343</v>
       </c>
@@ -3556,10 +3556,10 @@
       <c r="AT54" s="19"/>
     </row>
     <row r="55" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="42"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="20">
         <v>44343</v>
       </c>
@@ -3615,10 +3615,10 @@
       <c r="AT55" s="19"/>
     </row>
     <row r="56" spans="1:46" ht="32.25" customHeight="1">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="42"/>
+      <c r="B56" s="47"/>
       <c r="C56" s="20">
         <v>44344</v>
       </c>
@@ -3674,10 +3674,10 @@
       <c r="AT56" s="19"/>
     </row>
     <row r="57" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="38"/>
+      <c r="B57" s="43"/>
       <c r="C57" s="20">
         <v>44347</v>
       </c>
@@ -3733,10 +3733,10 @@
       <c r="AT57" s="19"/>
     </row>
     <row r="58" spans="1:46" ht="34.5" customHeight="1">
-      <c r="A58" s="41" t="s">
+      <c r="A58" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="42"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="20">
         <v>44347</v>
       </c>
@@ -3792,10 +3792,10 @@
       <c r="AT58" s="19"/>
     </row>
     <row r="59" spans="1:46" ht="31.5" customHeight="1">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="42"/>
+      <c r="B59" s="47"/>
       <c r="C59" s="20">
         <v>44350</v>
       </c>
@@ -3851,10 +3851,10 @@
       <c r="AT59" s="19"/>
     </row>
     <row r="60" spans="1:46">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="42"/>
+      <c r="B60" s="47"/>
       <c r="C60" s="20">
         <v>44351</v>
       </c>
@@ -3910,10 +3910,10 @@
       <c r="AT60" s="19"/>
     </row>
     <row r="61" spans="1:46" ht="42.75" customHeight="1">
-      <c r="A61" s="39" t="s">
+      <c r="A61" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="40"/>
+      <c r="B61" s="45"/>
       <c r="C61" s="23"/>
       <c r="D61" s="23"/>
       <c r="E61" s="23"/>
@@ -3960,10 +3960,10 @@
       <c r="AT61" s="15"/>
     </row>
     <row r="62" spans="1:46" ht="31.5" customHeight="1">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="38"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="20">
         <v>44354</v>
       </c>
@@ -4019,10 +4019,10 @@
       <c r="AT62" s="34"/>
     </row>
     <row r="63" spans="1:46" ht="36.75" customHeight="1">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="38"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="20">
         <v>44357</v>
       </c>
@@ -4078,10 +4078,10 @@
       <c r="AT63" s="34"/>
     </row>
     <row r="64" spans="1:46" ht="32.25" customHeight="1">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="38"/>
+      <c r="B64" s="43"/>
       <c r="C64" s="20">
         <v>44358</v>
       </c>
@@ -4137,10 +4137,10 @@
       <c r="AT64" s="34"/>
     </row>
     <row r="65" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="38"/>
+      <c r="B65" s="43"/>
       <c r="C65" s="20">
         <v>44362</v>
       </c>
@@ -4194,10 +4194,10 @@
       <c r="AT65" s="34"/>
     </row>
     <row r="66" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="38"/>
+      <c r="B66" s="43"/>
       <c r="C66" s="20">
         <v>44364</v>
       </c>
@@ -4253,10 +4253,10 @@
       <c r="AT66" s="34"/>
     </row>
     <row r="67" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="40"/>
+      <c r="B67" s="45"/>
       <c r="C67" s="23"/>
       <c r="D67" s="23"/>
       <c r="E67" s="23"/>
@@ -4303,10 +4303,10 @@
       <c r="AT67" s="15"/>
     </row>
     <row r="68" spans="1:46" ht="36" customHeight="1">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="38"/>
+      <c r="B68" s="43"/>
       <c r="C68" s="20">
         <v>44368</v>
       </c>
@@ -4362,10 +4362,10 @@
       <c r="AT68" s="22"/>
     </row>
     <row r="69" spans="1:46" ht="22.15" customHeight="1">
-      <c r="A69" s="37" t="s">
+      <c r="A69" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="38"/>
+      <c r="B69" s="43"/>
       <c r="C69" s="20">
         <v>44368</v>
       </c>
@@ -4477,6 +4477,45 @@
     <row r="71" spans="1:46" ht="28.9" customHeight="1"/>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A15:B15"/>
@@ -4493,45 +4532,6 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A64:B64"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>